<commit_message>
fix avoided cost of ng not in net annual revenues
</commit_message>
<xml_diff>
--- a/code/input_data/eia_aeo_industrial_sector_ng_prices.xlsx
+++ b/code/input_data/eia_aeo_industrial_sector_ng_prices.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="prices_division" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="map_census_division_state" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="state_prices" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="prices_division" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="map_census_division_state" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="state_prices" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -54,6 +54,11 @@
       <sz val="12"/>
     </font>
     <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
       <b val="1"/>
     </font>
   </fonts>
@@ -65,7 +70,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -106,6 +111,21 @@
       <top/>
       <bottom style="thin">
         <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -172,9 +192,12 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -597,10 +620,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -629,11 +652,6 @@
           <t>price 2022USD/MMBtu</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>price 2020USD/MMBtu</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -652,10 +670,6 @@
       <c r="D2" t="n">
         <v>8.235946</v>
       </c>
-      <c r="E2">
-        <f>D2/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -674,10 +688,6 @@
       <c r="D3" t="n">
         <v>5.928358</v>
       </c>
-      <c r="E3">
-        <f>D3/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -696,10 +706,6 @@
       <c r="D4" t="n">
         <v>5.580162</v>
       </c>
-      <c r="E4">
-        <f>D4/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -718,10 +724,6 @@
       <c r="D5" t="n">
         <v>4.283236</v>
       </c>
-      <c r="E5">
-        <f>D5/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -740,10 +742,6 @@
       <c r="D6" t="n">
         <v>5.053662</v>
       </c>
-      <c r="E6">
-        <f>D6/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -762,10 +760,6 @@
       <c r="D7" t="n">
         <v>3.824098</v>
       </c>
-      <c r="E7">
-        <f>D7/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -784,10 +778,6 @@
       <c r="D8" t="n">
         <v>6.189209</v>
       </c>
-      <c r="E8">
-        <f>D8/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -806,10 +796,6 @@
       <c r="D9" t="n">
         <v>4.591992</v>
       </c>
-      <c r="E9">
-        <f>D9/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -828,10 +814,6 @@
       <c r="D10" t="n">
         <v>5.223902</v>
       </c>
-      <c r="E10">
-        <f>D10/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -850,10 +832,6 @@
       <c r="D11" t="n">
         <v>4.016143</v>
       </c>
-      <c r="E11">
-        <f>D11/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -872,10 +850,6 @@
       <c r="D12" t="n">
         <v>6.192139</v>
       </c>
-      <c r="E12">
-        <f>D12/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -894,10 +868,6 @@
       <c r="D13" t="n">
         <v>4.917006</v>
       </c>
-      <c r="E13">
-        <f>D13/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -916,10 +886,6 @@
       <c r="D14" t="n">
         <v>5.556116</v>
       </c>
-      <c r="E14">
-        <f>D14/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -938,10 +904,6 @@
       <c r="D15" t="n">
         <v>4.117235</v>
       </c>
-      <c r="E15">
-        <f>D15/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -960,10 +922,6 @@
       <c r="D16" t="n">
         <v>4.996864</v>
       </c>
-      <c r="E16">
-        <f>D16/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -982,10 +940,6 @@
       <c r="D17" t="n">
         <v>3.776626</v>
       </c>
-      <c r="E17">
-        <f>D17/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1004,10 +958,6 @@
       <c r="D18" t="n">
         <v>4.464648</v>
       </c>
-      <c r="E18">
-        <f>D18/1.09</f>
-        <v/>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1025,10 +975,6 @@
       </c>
       <c r="D19" t="n">
         <v>3.344743</v>
-      </c>
-      <c r="E19">
-        <f>D19/1.09</f>
-        <v/>
       </c>
     </row>
   </sheetData>
@@ -1044,7 +990,7 @@
   </sheetPr>
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -1685,17 +1631,17 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>state</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>year</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>price 2020USD/MMBtu</t>
         </is>
@@ -1730,85 +1676,85 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>KY</t>
+          <t>AK</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>2024</v>
       </c>
       <c r="C4" t="n">
-        <v>4.636387155963303</v>
+        <v>5.680861467889908</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>KY</t>
+          <t>AK</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>2030</v>
       </c>
       <c r="C5" t="n">
-        <v>3.508346788990826</v>
+        <v>4.511014678899082</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>2024</v>
       </c>
       <c r="C6" t="n">
-        <v>4.636387155963303</v>
+        <v>4.792570642201834</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>AZ</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>2030</v>
       </c>
       <c r="C7" t="n">
-        <v>3.508346788990826</v>
+        <v>3.68453486238532</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>2024</v>
       </c>
       <c r="C8" t="n">
-        <v>4.636387155963303</v>
+        <v>4.096007339449542</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TN</t>
+          <t>AR</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>2030</v>
       </c>
       <c r="C9" t="n">
-        <v>3.508346788990826</v>
+        <v>3.068571559633027</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>AK</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1821,7 +1767,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AK</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1834,157 +1780,157 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2024</v>
       </c>
       <c r="C12" t="n">
-        <v>5.680861467889908</v>
+        <v>4.792570642201834</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CA</t>
+          <t>CO</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>2030</v>
       </c>
       <c r="C13" t="n">
-        <v>4.511014678899082</v>
+        <v>3.68453486238532</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>HI</t>
+          <t>CT</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>2024</v>
       </c>
       <c r="C14" t="n">
-        <v>5.680861467889908</v>
+        <v>7.55591376146789</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>HI</t>
+          <t>CT</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>2030</v>
       </c>
       <c r="C15" t="n">
-        <v>4.511014678899082</v>
+        <v>5.438860550458715</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>OR</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="B16" t="n">
         <v>2024</v>
       </c>
       <c r="C16" t="n">
-        <v>5.680861467889908</v>
+        <v>5.097354128440367</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>OR</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>2030</v>
       </c>
       <c r="C17" t="n">
-        <v>4.511014678899082</v>
+        <v>3.777279816513761</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WA</t>
+          <t>FL</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>2024</v>
       </c>
       <c r="C18" t="n">
-        <v>5.680861467889908</v>
+        <v>5.097354128440367</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>WA</t>
+          <t>FL</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>2030</v>
       </c>
       <c r="C19" t="n">
-        <v>4.511014678899082</v>
+        <v>3.777279816513761</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>GA</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>2024</v>
       </c>
       <c r="C20" t="n">
-        <v>4.792570642201834</v>
+        <v>5.097354128440367</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>AZ</t>
+          <t>GA</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>2030</v>
       </c>
       <c r="C21" t="n">
-        <v>3.68453486238532</v>
+        <v>3.777279816513761</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>HI</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>2024</v>
       </c>
       <c r="C22" t="n">
-        <v>4.792570642201834</v>
+        <v>5.680861467889908</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CO</t>
+          <t>HI</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>2030</v>
       </c>
       <c r="C23" t="n">
-        <v>3.68453486238532</v>
+        <v>4.511014678899082</v>
       </c>
     </row>
     <row r="24">
@@ -2016,137 +1962,137 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="B26" t="n">
         <v>2024</v>
       </c>
       <c r="C26" t="n">
-        <v>4.792570642201834</v>
+        <v>5.119414678899082</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="B27" t="n">
         <v>2030</v>
       </c>
       <c r="C27" t="n">
-        <v>3.68453486238532</v>
+        <v>3.929574311926605</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>NV</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="B28" t="n">
         <v>2024</v>
       </c>
       <c r="C28" t="n">
-        <v>4.792570642201834</v>
+        <v>5.119414678899082</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>NV</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="B29" t="n">
         <v>2030</v>
       </c>
       <c r="C29" t="n">
-        <v>3.68453486238532</v>
+        <v>3.929574311926605</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>NM</t>
+          <t>IA</t>
         </is>
       </c>
       <c r="B30" t="n">
         <v>2024</v>
       </c>
       <c r="C30" t="n">
-        <v>4.792570642201834</v>
+        <v>4.584278899082569</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>NM</t>
+          <t>IA</t>
         </is>
       </c>
       <c r="B31" t="n">
         <v>2030</v>
       </c>
       <c r="C31" t="n">
-        <v>3.68453486238532</v>
+        <v>3.464794495412844</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>UT</t>
+          <t>KS</t>
         </is>
       </c>
       <c r="B32" t="n">
         <v>2024</v>
       </c>
       <c r="C32" t="n">
-        <v>4.792570642201834</v>
+        <v>4.584278899082569</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>UT</t>
+          <t>KS</t>
         </is>
       </c>
       <c r="B33" t="n">
         <v>2030</v>
       </c>
       <c r="C33" t="n">
-        <v>3.68453486238532</v>
+        <v>3.464794495412844</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>WY</t>
+          <t>KY</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>2024</v>
       </c>
       <c r="C34" t="n">
-        <v>4.792570642201834</v>
+        <v>4.636387155963303</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>WY</t>
+          <t>KY</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>2030</v>
       </c>
       <c r="C35" t="n">
-        <v>3.68453486238532</v>
+        <v>3.508346788990826</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>LA</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -2159,7 +2105,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>AR</t>
+          <t>LA</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -2172,371 +2118,371 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>LA</t>
+          <t>ME</t>
         </is>
       </c>
       <c r="B38" t="n">
         <v>2024</v>
       </c>
       <c r="C38" t="n">
-        <v>4.096007339449542</v>
+        <v>7.55591376146789</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>LA</t>
+          <t>ME</t>
         </is>
       </c>
       <c r="B39" t="n">
         <v>2030</v>
       </c>
       <c r="C39" t="n">
-        <v>3.068571559633027</v>
+        <v>5.438860550458715</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>MD</t>
         </is>
       </c>
       <c r="B40" t="n">
         <v>2024</v>
       </c>
       <c r="C40" t="n">
-        <v>4.096007339449542</v>
+        <v>5.097354128440367</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>OK</t>
+          <t>MD</t>
         </is>
       </c>
       <c r="B41" t="n">
         <v>2030</v>
       </c>
       <c r="C41" t="n">
-        <v>3.068571559633027</v>
+        <v>3.777279816513761</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>TX</t>
+          <t>MA</t>
         </is>
       </c>
       <c r="B42" t="n">
         <v>2024</v>
       </c>
       <c r="C42" t="n">
-        <v>4.096007339449542</v>
+        <v>7.55591376146789</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>TX</t>
+          <t>MA</t>
         </is>
       </c>
       <c r="B43" t="n">
         <v>2030</v>
       </c>
       <c r="C43" t="n">
-        <v>3.068571559633027</v>
+        <v>5.438860550458715</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CT</t>
+          <t>MI</t>
         </is>
       </c>
       <c r="B44" t="n">
         <v>2024</v>
       </c>
       <c r="C44" t="n">
-        <v>7.55591376146789</v>
+        <v>5.119414678899082</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CT</t>
+          <t>MI</t>
         </is>
       </c>
       <c r="B45" t="n">
         <v>2030</v>
       </c>
       <c r="C45" t="n">
-        <v>5.438860550458715</v>
+        <v>3.929574311926605</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>ME</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="B46" t="n">
         <v>2024</v>
       </c>
       <c r="C46" t="n">
-        <v>7.55591376146789</v>
+        <v>4.584278899082569</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ME</t>
+          <t>MN</t>
         </is>
       </c>
       <c r="B47" t="n">
         <v>2030</v>
       </c>
       <c r="C47" t="n">
-        <v>5.438860550458715</v>
+        <v>3.464794495412844</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>2024</v>
       </c>
       <c r="C48" t="n">
-        <v>7.55591376146789</v>
+        <v>4.636387155963303</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>2030</v>
       </c>
       <c r="C49" t="n">
-        <v>5.438860550458715</v>
+        <v>3.508346788990826</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>NH</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>2024</v>
       </c>
       <c r="C50" t="n">
-        <v>7.55591376146789</v>
+        <v>4.584278899082569</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>NH</t>
+          <t>MO</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>2030</v>
       </c>
       <c r="C51" t="n">
-        <v>5.438860550458715</v>
+        <v>3.464794495412844</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>RI</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>2024</v>
       </c>
       <c r="C52" t="n">
-        <v>7.55591376146789</v>
+        <v>4.792570642201834</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>RI</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="B53" t="n">
         <v>2030</v>
       </c>
       <c r="C53" t="n">
-        <v>5.438860550458715</v>
+        <v>3.68453486238532</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>VT</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="B54" t="n">
         <v>2024</v>
       </c>
       <c r="C54" t="n">
-        <v>7.55591376146789</v>
+        <v>4.584278899082569</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>VT</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="B55" t="n">
         <v>2030</v>
       </c>
       <c r="C55" t="n">
-        <v>5.438860550458715</v>
+        <v>3.464794495412844</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>NV</t>
         </is>
       </c>
       <c r="B56" t="n">
         <v>2024</v>
       </c>
       <c r="C56" t="n">
-        <v>5.097354128440367</v>
+        <v>4.792570642201834</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>NV</t>
         </is>
       </c>
       <c r="B57" t="n">
         <v>2030</v>
       </c>
       <c r="C57" t="n">
-        <v>3.777279816513761</v>
+        <v>3.68453486238532</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>FL</t>
+          <t>NH</t>
         </is>
       </c>
       <c r="B58" t="n">
         <v>2024</v>
       </c>
       <c r="C58" t="n">
-        <v>5.097354128440367</v>
+        <v>7.55591376146789</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>FL</t>
+          <t>NH</t>
         </is>
       </c>
       <c r="B59" t="n">
         <v>2030</v>
       </c>
       <c r="C59" t="n">
-        <v>3.777279816513761</v>
+        <v>5.438860550458715</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="B60" t="n">
         <v>2024</v>
       </c>
       <c r="C60" t="n">
-        <v>5.097354128440367</v>
+        <v>5.678173394495412</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>GA</t>
+          <t>NJ</t>
         </is>
       </c>
       <c r="B61" t="n">
         <v>2030</v>
       </c>
       <c r="C61" t="n">
-        <v>3.777279816513761</v>
+        <v>4.212836697247706</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>MD</t>
+          <t>NM</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>2024</v>
       </c>
       <c r="C62" t="n">
-        <v>5.097354128440367</v>
+        <v>4.792570642201834</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>MD</t>
+          <t>NM</t>
         </is>
       </c>
       <c r="B63" t="n">
         <v>2030</v>
       </c>
       <c r="C63" t="n">
-        <v>3.777279816513761</v>
+        <v>3.68453486238532</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>2024</v>
       </c>
       <c r="C64" t="n">
-        <v>5.097354128440367</v>
+        <v>5.678173394495412</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>NY</t>
         </is>
       </c>
       <c r="B65" t="n">
         <v>2030</v>
       </c>
       <c r="C65" t="n">
-        <v>3.777279816513761</v>
+        <v>4.212836697247706</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -2549,7 +2495,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>SC</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -2562,189 +2508,189 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>ND</t>
         </is>
       </c>
       <c r="B68" t="n">
         <v>2024</v>
       </c>
       <c r="C68" t="n">
-        <v>5.097354128440367</v>
+        <v>4.584278899082569</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>VA</t>
+          <t>ND</t>
         </is>
       </c>
       <c r="B69" t="n">
         <v>2030</v>
       </c>
       <c r="C69" t="n">
-        <v>3.777279816513761</v>
+        <v>3.464794495412844</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>OH</t>
         </is>
       </c>
       <c r="B70" t="n">
         <v>2024</v>
       </c>
       <c r="C70" t="n">
-        <v>5.097354128440367</v>
+        <v>5.119414678899082</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>WV</t>
+          <t>OH</t>
         </is>
       </c>
       <c r="B71" t="n">
         <v>2030</v>
       </c>
       <c r="C71" t="n">
-        <v>3.777279816513761</v>
+        <v>3.929574311926605</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="B72" t="n">
         <v>2024</v>
       </c>
       <c r="C72" t="n">
-        <v>5.119414678899082</v>
+        <v>4.096007339449542</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>OK</t>
         </is>
       </c>
       <c r="B73" t="n">
         <v>2030</v>
       </c>
       <c r="C73" t="n">
-        <v>3.929574311926605</v>
+        <v>3.068571559633027</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="B74" t="n">
         <v>2024</v>
       </c>
       <c r="C74" t="n">
-        <v>5.119414678899082</v>
+        <v>5.680861467889908</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>OR</t>
         </is>
       </c>
       <c r="B75" t="n">
         <v>2030</v>
       </c>
       <c r="C75" t="n">
-        <v>3.929574311926605</v>
+        <v>4.511014678899082</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>MI</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="B76" t="n">
         <v>2024</v>
       </c>
       <c r="C76" t="n">
-        <v>5.119414678899082</v>
+        <v>5.678173394495412</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>MI</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="B77" t="n">
         <v>2030</v>
       </c>
       <c r="C77" t="n">
-        <v>3.929574311926605</v>
+        <v>4.212836697247706</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>OH</t>
+          <t>RI</t>
         </is>
       </c>
       <c r="B78" t="n">
         <v>2024</v>
       </c>
       <c r="C78" t="n">
-        <v>5.119414678899082</v>
+        <v>7.55591376146789</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>OH</t>
+          <t>RI</t>
         </is>
       </c>
       <c r="B79" t="n">
         <v>2030</v>
       </c>
       <c r="C79" t="n">
-        <v>3.929574311926605</v>
+        <v>5.438860550458715</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>WI</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="B80" t="n">
         <v>2024</v>
       </c>
       <c r="C80" t="n">
-        <v>5.119414678899082</v>
+        <v>5.097354128440367</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>WI</t>
+          <t>SC</t>
         </is>
       </c>
       <c r="B81" t="n">
         <v>2030</v>
       </c>
       <c r="C81" t="n">
-        <v>3.929574311926605</v>
+        <v>3.777279816513761</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>IA</t>
+          <t>SD</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -2757,7 +2703,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>IA</t>
+          <t>SD</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -2770,235 +2716,235 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>KS</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B84" t="n">
         <v>2024</v>
       </c>
       <c r="C84" t="n">
-        <v>4.584278899082569</v>
+        <v>4.636387155963303</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>KS</t>
+          <t>TN</t>
         </is>
       </c>
       <c r="B85" t="n">
         <v>2030</v>
       </c>
       <c r="C85" t="n">
-        <v>3.464794495412844</v>
+        <v>3.508346788990826</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>TX</t>
         </is>
       </c>
       <c r="B86" t="n">
         <v>2024</v>
       </c>
       <c r="C86" t="n">
-        <v>4.584278899082569</v>
+        <v>4.096007339449542</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>MN</t>
+          <t>TX</t>
         </is>
       </c>
       <c r="B87" t="n">
         <v>2030</v>
       </c>
       <c r="C87" t="n">
-        <v>3.464794495412844</v>
+        <v>3.068571559633027</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>UT</t>
         </is>
       </c>
       <c r="B88" t="n">
         <v>2024</v>
       </c>
       <c r="C88" t="n">
-        <v>4.584278899082569</v>
+        <v>4.792570642201834</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>MO</t>
+          <t>UT</t>
         </is>
       </c>
       <c r="B89" t="n">
         <v>2030</v>
       </c>
       <c r="C89" t="n">
-        <v>3.464794495412844</v>
+        <v>3.68453486238532</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>VT</t>
         </is>
       </c>
       <c r="B90" t="n">
         <v>2024</v>
       </c>
       <c r="C90" t="n">
-        <v>4.584278899082569</v>
+        <v>7.55591376146789</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>VT</t>
         </is>
       </c>
       <c r="B91" t="n">
         <v>2030</v>
       </c>
       <c r="C91" t="n">
-        <v>3.464794495412844</v>
+        <v>5.438860550458715</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="B92" t="n">
         <v>2024</v>
       </c>
       <c r="C92" t="n">
-        <v>4.584278899082569</v>
+        <v>5.097354128440367</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>ND</t>
+          <t>VA</t>
         </is>
       </c>
       <c r="B93" t="n">
         <v>2030</v>
       </c>
       <c r="C93" t="n">
-        <v>3.464794495412844</v>
+        <v>3.777279816513761</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>WA</t>
         </is>
       </c>
       <c r="B94" t="n">
         <v>2024</v>
       </c>
       <c r="C94" t="n">
-        <v>4.584278899082569</v>
+        <v>5.680861467889908</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>SD</t>
+          <t>WA</t>
         </is>
       </c>
       <c r="B95" t="n">
         <v>2030</v>
       </c>
       <c r="C95" t="n">
-        <v>3.464794495412844</v>
+        <v>4.511014678899082</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>WV</t>
         </is>
       </c>
       <c r="B96" t="n">
         <v>2024</v>
       </c>
       <c r="C96" t="n">
-        <v>5.678173394495412</v>
+        <v>5.097354128440367</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>NJ</t>
+          <t>WV</t>
         </is>
       </c>
       <c r="B97" t="n">
         <v>2030</v>
       </c>
       <c r="C97" t="n">
-        <v>4.212836697247706</v>
+        <v>3.777279816513761</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>WI</t>
         </is>
       </c>
       <c r="B98" t="n">
         <v>2024</v>
       </c>
       <c r="C98" t="n">
-        <v>5.678173394495412</v>
+        <v>5.119414678899082</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>NY</t>
+          <t>WI</t>
         </is>
       </c>
       <c r="B99" t="n">
         <v>2030</v>
       </c>
       <c r="C99" t="n">
-        <v>4.212836697247706</v>
+        <v>3.929574311926605</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>WY</t>
         </is>
       </c>
       <c r="B100" t="n">
         <v>2024</v>
       </c>
       <c r="C100" t="n">
-        <v>5.678173394495412</v>
+        <v>4.792570642201834</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>WY</t>
         </is>
       </c>
       <c r="B101" t="n">
         <v>2030</v>
       </c>
       <c r="C101" t="n">
-        <v>4.212836697247706</v>
+        <v>3.68453486238532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>